<commit_message>
can process both pdf and excel now!
but will still need a lot of tweaking for the code to be more robust
</commit_message>
<xml_diff>
--- a/aqs_bot/parts_extraction/input/drawing/01-E26VS691A003-00_170926_0209F.xlsx
+++ b/aqs_bot/parts_extraction/input/drawing/01-E26VS691A003-00_170926_0209F.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Darren Ho\Documents\GitHub\fyp\aqs_bot\parts_extraction\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Darren Ho\Documents\GitHub\fyp\aqs_bot\parts_extraction\input\drawing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{620F8C65-D4DB-4048-AD8F-8E684DCD7ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D6AF81C-EFDD-41FF-955C-4AEB3513F738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5385" yWindow="1140" windowWidth="16005" windowHeight="15915" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1380" yWindow="810" windowWidth="18195" windowHeight="17730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,9 +30,6 @@
     <t>PART DESCRIPTION</t>
   </si>
   <si>
-    <t>PART  NO / PART SPEC</t>
-  </si>
-  <si>
     <t>MA NO</t>
   </si>
   <si>
@@ -76,6 +73,9 @@
   </si>
   <si>
     <t>MM</t>
+  </si>
+  <si>
+    <t>PART NO / PART SPEC</t>
   </si>
 </sst>
 </file>
@@ -399,7 +399,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,36 +417,36 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="F2" s="1">
         <v>9</v>
@@ -454,19 +454,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="F3" s="1">
         <v>1</v>
@@ -474,19 +474,19 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1">
         <v>4160400</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F4" s="1">
         <v>1300</v>

</xml_diff>